<commit_message>
SAM sol results with CAIOS tariffs
</commit_message>
<xml_diff>
--- a/simulations/json/sol/sam_results.xlsx
+++ b/simulations/json/sol/sam_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\neup-ies\simulations\json\sol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03538FBB-4FB3-438E-8BBE-0D2E6F791D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE89EA6-86E5-4145-B914-7570B6A0784F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40455" yWindow="990" windowWidth="17250" windowHeight="9945" xr2:uid="{A007E866-B263-4FE2-B2F4-B3B424185BE8}"/>
+    <workbookView xWindow="29190" yWindow="2130" windowWidth="17280" windowHeight="9960" xr2:uid="{A007E866-B263-4FE2-B2F4-B3B424185BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="14">
   <si>
     <t>ppa (y1)</t>
   </si>
@@ -72,12 +72,18 @@
   <si>
     <t>Note: TES hours is in terms of cycle thermal power so in each optimal case we are storing about the same amount of receiver power</t>
   </si>
+  <si>
+    <t>Default Tariff Schedule</t>
+  </si>
+  <si>
+    <t>CAISO Tarriff Schedule</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +95,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,9 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF8FBA6-E8E6-4669-8C39-0CFAF02E2FC0}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,17 +466,26 @@
     <col min="3" max="3" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -467,8 +499,21 @@
         <f>B$12/B3*D$12</f>
         <v>163.92</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1">
+        <f>H$12/H3*J$12</f>
+        <v>163.92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -481,446 +526,833 @@
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
         <v>13.79</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>17.850000000000001</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>14.17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
         <v>11.67</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>14.9</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>11.83</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7">
         <v>10.62</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>13.27</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>10.54</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <v>10.27</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>12.57</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>9.98</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>10.35</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>12.6</v>
       </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
         <v>10.61</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>12.91</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>10.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="1">
         <v>2.4</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>136.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="3">
+        <v>136.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
       <c r="B14">
         <v>14.77</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>19.12</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>15.18</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
         <v>12.41</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>15.8</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>12.55</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
       <c r="B16">
         <v>11.12</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>13.86</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>11.01</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
       <c r="B17">
         <v>10.4</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>12.58</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>9.99</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
       <c r="B18">
         <v>10.039999999999999</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>11.87</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>9.42</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>8</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10</v>
       </c>
       <c r="B19">
         <v>9.9600000000000009</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>11.64</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>9.24</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="1">
         <v>2.8</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <f>B$12/B21*D$12</f>
         <v>117.08571428571429</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="3">
+        <f>H$12/H21*J$12</f>
+        <v>117.08571428571429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="C22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
       <c r="B23">
         <v>15.84</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>20.5</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>16.28</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>36.9</v>
+      </c>
+      <c r="I23" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="J23" s="2">
+        <v>16.28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24">
         <v>13.27</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>16.89</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>13.41</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>21.67</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25">
         <v>11.79</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>14.66</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>11.64</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>15.71</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
       <c r="B26">
         <v>10.9</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>13.13</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>10.43</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>13.24</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
       </c>
       <c r="B27">
         <v>10.33</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>12.09</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <v>11.95</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
       <c r="B28">
         <v>9.9700000000000006</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>11.42</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>9.07</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28">
+        <v>11.26</v>
+      </c>
+      <c r="I28" s="2">
+        <v>11.42</v>
+      </c>
+      <c r="J28" s="2">
+        <v>9.07</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>12</v>
       </c>
       <c r="B29">
         <v>9.7899999999999991</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>11.08</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>12</v>
+      </c>
+      <c r="H29">
+        <v>10.9</v>
+      </c>
+      <c r="I29" s="2">
+        <v>11.08</v>
+      </c>
+      <c r="J29" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>14</v>
       </c>
       <c r="B30">
         <v>9.84</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>11.1</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>8.82</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>14</v>
+      </c>
+      <c r="H30">
+        <v>10.9</v>
+      </c>
+      <c r="I30" s="2">
+        <v>11.1</v>
+      </c>
+      <c r="J30" s="2">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1">
         <v>3.2</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="3">
         <f>B$12/B32*D$12</f>
         <v>102.44999999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32" s="3">
+        <f>H$12/H32*J$12</f>
+        <v>102.44999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="C33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>10</v>
       </c>
       <c r="B34">
         <v>10.32</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>11.74</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>9.32</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>10</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12</v>
       </c>
       <c r="B35">
         <v>9.94</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>11.1</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="2">
         <v>8.82</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>12</v>
+      </c>
+      <c r="H35">
+        <v>10.73</v>
+      </c>
+      <c r="I35" s="2">
+        <v>11.1</v>
+      </c>
+      <c r="J35" s="2">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>14</v>
       </c>
       <c r="B36">
         <v>9.8000000000000007</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>10.86</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="2">
         <v>8.6199999999999992</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <v>14</v>
+      </c>
+      <c r="H36">
+        <v>10.35</v>
+      </c>
+      <c r="I36" s="2">
+        <v>10.86</v>
+      </c>
+      <c r="J36" s="2">
+        <v>8.6199999999999992</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>16</v>
       </c>
       <c r="B37">
         <v>9.8800000000000008</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>10.94</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="2">
         <v>8.68</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="G37">
+        <v>16</v>
+      </c>
+      <c r="H37">
+        <v>10.41</v>
+      </c>
+      <c r="I37" s="2">
+        <v>10.94</v>
+      </c>
+      <c r="J37" s="2">
+        <v>8.68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J39" s="3">
+        <f>H$12/H39*J$12</f>
+        <v>91.066666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <v>12</v>
+      </c>
+      <c r="H41">
+        <v>10.97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <v>14</v>
+      </c>
+      <c r="H42">
+        <v>10.34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>16</v>
+      </c>
+      <c r="H43">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G44">
+        <v>18</v>
+      </c>
+      <c r="H44">
+        <v>10.28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="1">
+        <v>4</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J46" s="3">
+        <f>H$12/H46*J$12</f>
+        <v>81.96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G48">
+        <v>16</v>
+      </c>
+      <c r="H48">
+        <v>10.63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <v>18</v>
+      </c>
+      <c r="H49">
+        <v>10.58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <v>20</v>
+      </c>
+      <c r="H50">
+        <v>10.67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="1" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>